<commit_message>
- Working in Issue #4
</commit_message>
<xml_diff>
--- a/testes2/nomesatp.xlsx
+++ b/testes2/nomesatp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="188">
   <si>
     <t>ATP</t>
   </si>
@@ -25,9 +25,6 @@
     <t>ONS nº</t>
   </si>
   <si>
-    <t>TERRA</t>
-  </si>
-  <si>
     <t>IVP76</t>
   </si>
   <si>
@@ -551,6 +548,36 @@
   </si>
   <si>
     <t>NSR52</t>
+  </si>
+  <si>
+    <t>SM323</t>
+  </si>
+  <si>
+    <t>SM369</t>
+  </si>
+  <si>
+    <t>MA323</t>
+  </si>
+  <si>
+    <t>GARA1</t>
+  </si>
+  <si>
+    <t>GARA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMARIA3 230 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMARIA3  69 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACAMB 3 230 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARABI II525 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARABI  525 </t>
   </si>
 </sst>
 </file>
@@ -1397,10 +1424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,1007 +1448,1048 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>177</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>7752</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>6030</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3">
-        <v>7747</v>
+        <v>7719</v>
+      </c>
+      <c r="C3">
+        <v>6050</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>6253</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>175</v>
+      </c>
+      <c r="C4">
+        <v>6092</v>
+      </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B5">
-        <v>6824</v>
+        <v>7751</v>
+      </c>
+      <c r="C5">
+        <v>6129</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6">
-        <v>6826</v>
+        <v>114</v>
+      </c>
+      <c r="C6">
+        <v>6229</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7">
-        <v>6627</v>
+        <v>171</v>
+      </c>
+      <c r="C7">
+        <v>6350</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>3696</v>
+        <v>166</v>
+      </c>
+      <c r="C8">
+        <v>6360</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B9">
-        <v>6200</v>
+        <v>7766</v>
+      </c>
+      <c r="C9">
+        <v>6395</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10">
-        <v>7742</v>
+        <v>182</v>
+      </c>
+      <c r="C10">
+        <v>6499</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>6211</v>
+        <v>181</v>
+      </c>
+      <c r="C11">
+        <v>6500</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>6224</v>
+        <v>115</v>
+      </c>
+      <c r="C12">
+        <v>6543</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <v>6223</v>
+        <v>173</v>
+      </c>
+      <c r="C13">
+        <v>6603</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>6217</v>
+        <v>117</v>
+      </c>
+      <c r="C14">
+        <v>6604</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15">
-        <v>6615</v>
+        <v>134</v>
+      </c>
+      <c r="C15">
+        <v>6658</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16">
-        <v>7723</v>
+        <v>120</v>
+      </c>
+      <c r="C16">
+        <v>28066</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17">
-        <v>6626</v>
+        <v>122</v>
+      </c>
+      <c r="C17">
+        <v>28102</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18">
-        <v>6762</v>
+        <v>124</v>
+      </c>
+      <c r="C18">
+        <v>28127</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19">
-        <v>7751</v>
+        <v>164</v>
       </c>
       <c r="C19">
-        <v>6129</v>
+        <v>28195</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20">
-        <v>6617</v>
+        <v>126</v>
+      </c>
+      <c r="C20">
+        <v>28196</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21">
-        <v>7917</v>
+        <v>127</v>
+      </c>
+      <c r="C21">
+        <v>28200</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22">
-        <v>7926</v>
+        <v>178</v>
+      </c>
+      <c r="C22">
+        <v>28230</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23">
-        <v>7928</v>
+        <v>179</v>
+      </c>
+      <c r="C23">
+        <v>28232</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24">
-        <v>44657</v>
+        <v>169</v>
+      </c>
+      <c r="C24">
+        <v>28245</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25">
-        <v>6761</v>
+        <v>128</v>
+      </c>
+      <c r="C25">
+        <v>28246</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26">
-        <v>6108</v>
+        <v>129</v>
+      </c>
+      <c r="C26">
+        <v>28250</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <v>6244</v>
+        <v>131</v>
+      </c>
+      <c r="C27">
+        <v>28280</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28">
-        <v>6664</v>
+        <v>133</v>
+      </c>
+      <c r="C28">
+        <v>28580</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29">
-        <v>50213</v>
+        <v>180</v>
+      </c>
+      <c r="C29">
+        <v>28651</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B30">
-        <v>6111</v>
+        <v>7747</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B31">
-        <v>6110</v>
-      </c>
+        <v>6253</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>123</v>
-      </c>
-      <c r="C32">
-        <v>28102</v>
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>6824</v>
       </c>
       <c r="D32" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B33">
-        <v>83001</v>
+        <v>6826</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B34">
-        <v>43351</v>
+        <v>6627</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>174</v>
-      </c>
-      <c r="C35">
-        <v>6603</v>
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>3696</v>
       </c>
       <c r="D35" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36">
-        <v>6604</v>
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>6200</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B37">
-        <v>7833</v>
+        <v>7742</v>
       </c>
       <c r="D37" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38">
-        <v>6229</v>
+        <v>19</v>
+      </c>
+      <c r="B38">
+        <v>6211</v>
       </c>
       <c r="D38" t="s">
-        <v>161</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B39">
-        <v>6268</v>
+        <v>6224</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B40">
-        <v>3654</v>
+        <v>6223</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B41">
-        <v>6121</v>
+        <v>6217</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B42">
-        <v>6162</v>
+        <v>6762</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B43">
-        <v>6160</v>
+        <v>44657</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B44">
-        <v>6142</v>
+        <v>6615</v>
       </c>
       <c r="D44" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B45">
-        <v>7802</v>
+        <v>6617</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B46">
-        <v>6132</v>
+        <v>7723</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B47">
-        <v>6306</v>
+        <v>7917</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>135</v>
-      </c>
-      <c r="C48">
-        <v>6658</v>
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>7926</v>
       </c>
       <c r="D48" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B49">
-        <v>7762</v>
+        <v>7928</v>
       </c>
       <c r="D49" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50">
-        <v>28127</v>
+        <v>35</v>
+      </c>
+      <c r="B50">
+        <v>6626</v>
       </c>
       <c r="D50" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B51">
-        <v>7719</v>
-      </c>
-      <c r="C51">
-        <v>6050</v>
+        <v>6108</v>
       </c>
       <c r="D51" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52">
-        <v>6092</v>
+        <v>23</v>
+      </c>
+      <c r="B52">
+        <v>6244</v>
       </c>
       <c r="D52" t="s">
-        <v>177</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>116</v>
-      </c>
-      <c r="C53">
-        <v>6543</v>
+        <v>37</v>
+      </c>
+      <c r="B53">
+        <v>6664</v>
       </c>
       <c r="D53" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>68</v>
       </c>
       <c r="B54">
-        <v>7752</v>
-      </c>
-      <c r="C54">
-        <v>6030</v>
+        <v>83001</v>
       </c>
       <c r="D54" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B55">
-        <v>6731</v>
+        <v>6110</v>
       </c>
       <c r="D55" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B56">
-        <v>7015</v>
+        <v>50213</v>
       </c>
       <c r="D56" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="B57">
-        <v>7809</v>
+        <v>6111</v>
       </c>
       <c r="D57" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="B58">
-        <v>6276</v>
+        <v>43351</v>
       </c>
       <c r="D58" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B59">
-        <v>6171</v>
+        <v>7833</v>
       </c>
       <c r="D59" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B60">
-        <v>6274</v>
+        <v>6268</v>
       </c>
       <c r="D60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B61">
-        <v>6281</v>
+        <v>3654</v>
       </c>
       <c r="D61" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62">
-        <v>28200</v>
+        <v>9</v>
+      </c>
+      <c r="B62">
+        <v>6121</v>
       </c>
       <c r="D62" t="s">
-        <v>163</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B63">
-        <v>7820</v>
+        <v>7802</v>
       </c>
       <c r="D63" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B64">
-        <v>7766</v>
-      </c>
-      <c r="C64">
-        <v>6395</v>
+        <v>6142</v>
       </c>
       <c r="D64" t="s">
-        <v>159</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B65">
-        <v>6757</v>
+        <v>6162</v>
       </c>
       <c r="D65" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>134</v>
-      </c>
-      <c r="C66">
-        <v>28580</v>
+        <v>12</v>
+      </c>
+      <c r="B66">
+        <v>6160</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>170</v>
-      </c>
-      <c r="C67">
-        <v>28245</v>
+        <v>10</v>
+      </c>
+      <c r="B67">
+        <v>6132</v>
       </c>
       <c r="D67" t="s">
-        <v>171</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>129</v>
-      </c>
-      <c r="C68">
-        <v>28246</v>
+        <v>31</v>
+      </c>
+      <c r="B68">
+        <v>6306</v>
       </c>
       <c r="D68" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>165</v>
-      </c>
-      <c r="C69">
-        <v>28195</v>
+        <v>53</v>
+      </c>
+      <c r="B69">
+        <v>7762</v>
       </c>
       <c r="D69" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
-      </c>
-      <c r="C70">
-        <v>28196</v>
+        <v>56</v>
+      </c>
+      <c r="B70">
+        <v>7809</v>
       </c>
       <c r="D70" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>167</v>
-      </c>
-      <c r="C71">
-        <v>6360</v>
+        <v>38</v>
+      </c>
+      <c r="B71">
+        <v>6731</v>
       </c>
       <c r="D71" t="s">
-        <v>168</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>172</v>
-      </c>
-      <c r="C72">
-        <v>6350</v>
+        <v>47</v>
+      </c>
+      <c r="B72">
+        <v>7015</v>
       </c>
       <c r="D72" t="s">
-        <v>173</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B73">
-        <v>6180</v>
+        <v>6276</v>
       </c>
       <c r="D73" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B74">
-        <v>6181</v>
+        <v>6171</v>
       </c>
       <c r="D74" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75">
-        <v>28066</v>
+        <v>26</v>
+      </c>
+      <c r="B75">
+        <v>6274</v>
       </c>
       <c r="D75" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B76">
-        <v>6185</v>
+        <v>6281</v>
       </c>
       <c r="D76" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="B77">
-        <v>7823</v>
+        <v>6180</v>
       </c>
       <c r="D77" t="s">
-        <v>156</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B78">
-        <v>6763</v>
+        <v>6181</v>
       </c>
       <c r="D78" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="B79">
-        <v>6764</v>
+        <v>6185</v>
       </c>
       <c r="D79" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="B80">
-        <v>8800</v>
+        <v>6757</v>
       </c>
       <c r="D80" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B81">
-        <v>44841</v>
+        <v>7823</v>
       </c>
       <c r="D81" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>130</v>
-      </c>
-      <c r="C82">
-        <v>28250</v>
+        <v>40</v>
+      </c>
+      <c r="B82">
+        <v>6761</v>
       </c>
       <c r="D82" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B83">
-        <v>6091</v>
+        <v>6763</v>
       </c>
       <c r="D83" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B84">
-        <v>6293</v>
+        <v>6764</v>
       </c>
       <c r="D84" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B85">
-        <v>6295</v>
+        <v>7820</v>
       </c>
       <c r="D85" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B86">
-        <v>99137</v>
+        <v>8800</v>
       </c>
       <c r="D86" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B87">
-        <v>6616</v>
+        <v>44841</v>
       </c>
       <c r="D87" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B88">
-        <v>6870</v>
+        <v>99137</v>
       </c>
       <c r="D88" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>132</v>
-      </c>
-      <c r="C89">
-        <v>28280</v>
+        <v>30</v>
+      </c>
+      <c r="B89">
+        <v>6295</v>
       </c>
       <c r="D89" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B90">
+        <v>6293</v>
+      </c>
+      <c r="D90" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>6091</v>
+      </c>
+      <c r="D91" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92">
+        <v>6616</v>
+      </c>
+      <c r="D92" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93">
+        <v>6870</v>
+      </c>
+      <c r="D93" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>69</v>
+      </c>
+      <c r="B94">
         <v>84000</v>
       </c>
-      <c r="D90" t="s">
-        <v>113</v>
+      <c r="D94" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:D89">
-    <sortCondition ref="D3:D89"/>
+  <sortState ref="A2:D94">
+    <sortCondition ref="C2:C94"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>